<commit_message>
mostly contact angle stuff
</commit_message>
<xml_diff>
--- a/SAMs/data/sample1.xlsx
+++ b/SAMs/data/sample1.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SAKI\Documents\GitHub\FoPra_SoSe16\SAMs\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7485" windowHeight="7013"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="25440" windowHeight="14440"/>
   </bookViews>
   <sheets>
     <sheet name="sample1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="130000"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -57,8 +57,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -650,51 +656,51 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - アクセント 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - アクセント 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - アクセント 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - アクセント 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - アクセント 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - アクセント 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - アクセント 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - アクセント 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - アクセント 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - アクセント 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - アクセント 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - アクセント 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - アクセント 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - アクセント 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - アクセント 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - アクセント 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - アクセント 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - アクセント 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="アクセント 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="アクセント 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="アクセント 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="アクセント 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="アクセント 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="アクセント 6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="タイトル" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="チェック セル" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="どちらでもない" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="メモ" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="リンク セル" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="悪い" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="計算" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="警告文" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="見出し 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="見出し 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="見出し 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="見出し 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="集計" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="出力" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="説明文" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="入力" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
-    <cellStyle name="良い" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent1 - 20%" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="Accent1 - 40%" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="Accent1 - 60%" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent2 - 20%" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="Accent2 - 40%" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="Accent2 - 60%" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent3 - 20%" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="Accent3 - 40%" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="Accent3 - 60%" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent4 - 20%" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="Accent4 - 40%" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="Accent4 - 60%" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent5 - 20%" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="Accent5 - 40%" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="Accent5 - 60%" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Accent6 - 20%" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="Accent6 - 40%" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="Accent6 - 60%" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Sheet Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -749,7 +755,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -801,7 +807,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -995,53 +1001,54 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1058,7 +1065,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1075,7 +1082,7 @@
         <v>14.53</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1092,7 +1099,7 @@
         <v>14.98</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.7">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1109,7 +1116,7 @@
         <v>15.04</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.7">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1126,7 +1133,7 @@
         <v>14.38</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.7">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1143,15 +1150,26 @@
         <v>15.27</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:5">
       <c r="B14">
         <f>AVERAGE(B9:B13)</f>
         <v>61.71</v>
       </c>
     </row>
+    <row r="16" spans="1:5">
+      <c r="B16">
+        <f>STDEV(B9:B13)</f>
+        <v>3.3121141284683335</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>